<commit_message>
Fixing output files, scr 159
- Also adding statistics
- Also knitting result file
</commit_message>
<xml_diff>
--- a/Data/159_df_meta1.xlsx
+++ b/Data/159_df_meta1.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB557"/>
+  <dimension ref="A1:AC557"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -498,6 +498,11 @@
           <t>other</t>
         </is>
       </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>altitude_ie</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2">
@@ -18641,7 +18646,7 @@
         <v>-6.35</v>
       </c>
       <c r="F187">
-        <v>133</v>
+        <v>133.1</v>
       </c>
       <c r="G187" t="inlineStr">
         <is>
@@ -18716,6 +18721,9 @@
       </c>
       <c r="AB187">
         <v>0.035</v>
+      </c>
+      <c r="AC187">
+        <v>133.1</v>
       </c>
     </row>
     <row r="188">
@@ -18739,7 +18747,7 @@
         <v>-6.383333</v>
       </c>
       <c r="F188">
-        <v>133</v>
+        <v>133.1</v>
       </c>
       <c r="G188" t="inlineStr">
         <is>
@@ -18760,6 +18768,9 @@
         <is>
           <t>Core</t>
         </is>
+      </c>
+      <c r="AC188">
+        <v>133.1</v>
       </c>
     </row>
     <row r="189">
@@ -18783,7 +18794,7 @@
         <v>-6.35</v>
       </c>
       <c r="F189">
-        <v>133</v>
+        <v>133.1</v>
       </c>
       <c r="G189" t="inlineStr">
         <is>
@@ -18804,6 +18815,9 @@
         <is>
           <t>Core</t>
         </is>
+      </c>
+      <c r="AC189">
+        <v>133.1</v>
       </c>
     </row>
     <row r="190">
@@ -18827,7 +18841,7 @@
         <v>-6.35</v>
       </c>
       <c r="F190">
-        <v>133</v>
+        <v>133.1</v>
       </c>
       <c r="G190" t="inlineStr">
         <is>
@@ -18848,6 +18862,9 @@
         <is>
           <t>Core</t>
         </is>
+      </c>
+      <c r="AC190">
+        <v>133.1</v>
       </c>
     </row>
     <row r="191">
@@ -18871,7 +18888,7 @@
         <v>-9.541</v>
       </c>
       <c r="F191">
-        <v>48</v>
+        <v>47.5</v>
       </c>
       <c r="G191" t="inlineStr">
         <is>
@@ -18946,6 +18963,9 @@
       </c>
       <c r="AB191">
         <v>0.024</v>
+      </c>
+      <c r="AC191">
+        <v>47.5</v>
       </c>
     </row>
     <row r="192">
@@ -18969,7 +18989,7 @@
         <v>-9.533333000000001</v>
       </c>
       <c r="F192">
-        <v>48</v>
+        <v>47.5</v>
       </c>
       <c r="G192" t="inlineStr">
         <is>
@@ -18990,6 +19010,9 @@
         <is>
           <t>Core</t>
         </is>
+      </c>
+      <c r="AC192">
+        <v>47.5</v>
       </c>
     </row>
     <row r="193">
@@ -19013,7 +19036,7 @@
         <v>-9.533333000000001</v>
       </c>
       <c r="F193">
-        <v>48</v>
+        <v>47.5</v>
       </c>
       <c r="G193" t="inlineStr">
         <is>
@@ -19034,6 +19057,9 @@
         <is>
           <t>Core</t>
         </is>
+      </c>
+      <c r="AC193">
+        <v>47.5</v>
       </c>
     </row>
     <row r="194">
@@ -19056,6 +19082,9 @@
       <c r="E194">
         <v>-7.95363</v>
       </c>
+      <c r="F194">
+        <v>45.3</v>
+      </c>
       <c r="G194" t="inlineStr">
         <is>
           <t>Europe</t>
@@ -19129,6 +19158,9 @@
       </c>
       <c r="AB194">
         <v>0.129</v>
+      </c>
+      <c r="AC194">
+        <v>45.3</v>
       </c>
     </row>
     <row r="195">
@@ -19151,6 +19183,9 @@
       <c r="E195">
         <v>-7.7</v>
       </c>
+      <c r="F195">
+        <v>45.3</v>
+      </c>
       <c r="G195" t="inlineStr">
         <is>
           <t>Europe</t>
@@ -19170,6 +19205,9 @@
         <is>
           <t>Core</t>
         </is>
+      </c>
+      <c r="AC195">
+        <v>45.3</v>
       </c>
     </row>
     <row r="196">
@@ -19192,6 +19230,9 @@
       <c r="E196">
         <v>-7.7</v>
       </c>
+      <c r="F196">
+        <v>45.3</v>
+      </c>
       <c r="G196" t="inlineStr">
         <is>
           <t>Europe</t>
@@ -19211,6 +19252,9 @@
         <is>
           <t>Core</t>
         </is>
+      </c>
+      <c r="AC196">
+        <v>45.3</v>
       </c>
     </row>
     <row r="197">
@@ -19233,6 +19277,9 @@
       <c r="E197">
         <v>-8.103999999999999</v>
       </c>
+      <c r="F197">
+        <v>88.59999999999999</v>
+      </c>
       <c r="G197" t="inlineStr">
         <is>
           <t>Europe</t>
@@ -19306,6 +19353,9 @@
       </c>
       <c r="AB197">
         <v>0.041</v>
+      </c>
+      <c r="AC197">
+        <v>88.59999999999999</v>
       </c>
     </row>
     <row r="198">
@@ -19328,6 +19378,9 @@
       <c r="E198">
         <v>-9.45429</v>
       </c>
+      <c r="F198">
+        <v>37.4</v>
+      </c>
       <c r="G198" t="inlineStr">
         <is>
           <t>Europe</t>
@@ -19401,6 +19454,9 @@
       </c>
       <c r="AB198">
         <v>3.325</v>
+      </c>
+      <c r="AC198">
+        <v>37.4</v>
       </c>
     </row>
     <row r="199">
@@ -19423,6 +19479,9 @@
       <c r="E199">
         <v>-10.05228</v>
       </c>
+      <c r="F199">
+        <v>209.3</v>
+      </c>
       <c r="G199" t="inlineStr">
         <is>
           <t>Europe</t>
@@ -19496,6 +19555,9 @@
       </c>
       <c r="AB199">
         <v>0</v>
+      </c>
+      <c r="AC199">
+        <v>209.3</v>
       </c>
     </row>
     <row r="200">
@@ -19518,6 +19580,9 @@
       <c r="E200">
         <v>-6.27918</v>
       </c>
+      <c r="F200">
+        <v>204.3</v>
+      </c>
       <c r="G200" t="inlineStr">
         <is>
           <t>Europe</t>
@@ -19591,6 +19656,9 @@
       </c>
       <c r="AB200">
         <v>0.958</v>
+      </c>
+      <c r="AC200">
+        <v>204.3</v>
       </c>
     </row>
     <row r="201">
@@ -19613,6 +19681,9 @@
       <c r="E201">
         <v>-9.304869999999999</v>
       </c>
+      <c r="F201">
+        <v>86.40000000000001</v>
+      </c>
       <c r="G201" t="inlineStr">
         <is>
           <t>Europe</t>
@@ -19686,6 +19757,9 @@
       </c>
       <c r="AB201">
         <v>1.593</v>
+      </c>
+      <c r="AC201">
+        <v>86.40000000000001</v>
       </c>
     </row>
     <row r="202">
@@ -19708,6 +19782,9 @@
       <c r="E202">
         <v>-8.85182</v>
       </c>
+      <c r="F202">
+        <v>183.2</v>
+      </c>
       <c r="G202" t="inlineStr">
         <is>
           <t>Europe</t>
@@ -19781,6 +19858,9 @@
       </c>
       <c r="AB202">
         <v>2.479</v>
+      </c>
+      <c r="AC202">
+        <v>183.2</v>
       </c>
     </row>
     <row r="203">
@@ -19803,6 +19883,9 @@
       <c r="E203">
         <v>-10.00595</v>
       </c>
+      <c r="F203">
+        <v>14.4</v>
+      </c>
       <c r="G203" t="inlineStr">
         <is>
           <t>Europe</t>
@@ -19876,6 +19959,9 @@
       </c>
       <c r="AB203">
         <v>14.536</v>
+      </c>
+      <c r="AC203">
+        <v>14.4</v>
       </c>
     </row>
     <row r="204">
@@ -19898,6 +19984,9 @@
       <c r="E204">
         <v>-9.786569999999999</v>
       </c>
+      <c r="F204">
+        <v>35.1</v>
+      </c>
       <c r="G204" t="inlineStr">
         <is>
           <t>Europe</t>
@@ -19971,6 +20060,9 @@
       </c>
       <c r="AB204">
         <v>1.431</v>
+      </c>
+      <c r="AC204">
+        <v>35.1</v>
       </c>
     </row>
     <row r="205">
@@ -19993,6 +20085,9 @@
       <c r="E205">
         <v>-9.54759</v>
       </c>
+      <c r="F205">
+        <v>36.2</v>
+      </c>
       <c r="G205" t="inlineStr">
         <is>
           <t>Europe</t>
@@ -20066,6 +20161,9 @@
       </c>
       <c r="AB205">
         <v>7.525</v>
+      </c>
+      <c r="AC205">
+        <v>36.2</v>
       </c>
     </row>
     <row r="206">
@@ -20088,6 +20186,9 @@
       <c r="E206">
         <v>-9.22064</v>
       </c>
+      <c r="F206">
+        <v>168.7</v>
+      </c>
       <c r="G206" t="inlineStr">
         <is>
           <t>Europe</t>
@@ -20161,6 +20262,9 @@
       </c>
       <c r="AB206">
         <v>0</v>
+      </c>
+      <c r="AC206">
+        <v>168.7</v>
       </c>
     </row>
     <row r="207">
@@ -20183,6 +20287,9 @@
       <c r="E207">
         <v>-9.588150000000001</v>
       </c>
+      <c r="F207">
+        <v>20</v>
+      </c>
       <c r="G207" t="inlineStr">
         <is>
           <t>Europe</t>
@@ -20256,6 +20363,9 @@
       </c>
       <c r="AB207">
         <v>0.905</v>
+      </c>
+      <c r="AC207">
+        <v>20</v>
       </c>
     </row>
     <row r="208">

</xml_diff>